<commit_message>
update 20220705 17:25 by xhx
</commit_message>
<xml_diff>
--- a/rules/rules.xlsx
+++ b/rules/rules.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20338"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B880CE4C-A531-4F8F-994F-8394A8728A0B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7905835-6979-43B8-A38A-6A776940A44B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -446,7 +446,7 @@
   <dimension ref="A1:I52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -507,7 +507,7 @@
         <v>4.0599999999999996</v>
       </c>
       <c r="F2" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G2" s="2">
         <v>0</v>
@@ -536,7 +536,7 @@
         <v>8.1199999999999992</v>
       </c>
       <c r="F3" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G3" s="2">
         <v>0</v>
@@ -565,7 +565,7 @@
         <v>16.239999999999998</v>
       </c>
       <c r="F4" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G4" s="2">
         <v>0</v>
@@ -594,7 +594,7 @@
         <v>32.479999999999997</v>
       </c>
       <c r="F5" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G5" s="2">
         <v>0</v>
@@ -623,7 +623,7 @@
         <v>4.0599999999999996</v>
       </c>
       <c r="F6" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G6" s="2">
         <v>0</v>
@@ -652,7 +652,7 @@
         <v>8.1199999999999992</v>
       </c>
       <c r="F7" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G7" s="2">
         <v>0</v>
@@ -681,7 +681,7 @@
         <v>16.239999999999998</v>
       </c>
       <c r="F8" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G8" s="2">
         <v>0</v>
@@ -710,7 +710,7 @@
         <v>32.479999999999997</v>
       </c>
       <c r="F9" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G9" s="2">
         <v>0</v>
@@ -739,7 +739,7 @@
         <v>4.0599999999999996</v>
       </c>
       <c r="F10" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G10" s="2">
         <v>0</v>
@@ -768,7 +768,7 @@
         <v>4.0599999999999996</v>
       </c>
       <c r="F11" s="2">
-        <v>2</v>
+        <v>50</v>
       </c>
       <c r="G11" s="2">
         <v>0</v>
@@ -797,7 +797,7 @@
         <v>4.0599999999999996</v>
       </c>
       <c r="F12" s="2">
-        <v>3</v>
+        <v>100</v>
       </c>
       <c r="G12" s="2">
         <v>0</v>
@@ -826,7 +826,7 @@
         <v>4</v>
       </c>
       <c r="F13" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G13" s="2">
         <v>0</v>
@@ -855,7 +855,7 @@
         <v>4.01</v>
       </c>
       <c r="F14" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G14" s="2">
         <v>0</v>
@@ -884,7 +884,7 @@
         <v>4.0199999999999996</v>
       </c>
       <c r="F15" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G15" s="2">
         <v>0</v>
@@ -913,7 +913,7 @@
         <v>4.03</v>
       </c>
       <c r="F16" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G16" s="2">
         <v>0</v>
@@ -942,7 +942,7 @@
         <v>4.0599999999999996</v>
       </c>
       <c r="F17" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G17" s="2">
         <v>0</v>
@@ -971,7 +971,7 @@
         <v>4</v>
       </c>
       <c r="F18" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G18" s="2">
         <v>0</v>
@@ -1000,7 +1000,7 @@
         <v>4.0599999999999996</v>
       </c>
       <c r="F19" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G19" s="2">
         <v>0</v>
@@ -1029,7 +1029,7 @@
         <v>0</v>
       </c>
       <c r="F20" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G20" s="2">
         <v>246.30539999999999</v>
@@ -1058,7 +1058,7 @@
         <v>4</v>
       </c>
       <c r="F21" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G21" s="2">
         <v>0</v>
@@ -1087,7 +1087,7 @@
         <v>4.01</v>
       </c>
       <c r="F22" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G22" s="2">
         <v>0</v>
@@ -1116,7 +1116,7 @@
         <v>4.0199999999999996</v>
       </c>
       <c r="F23" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G23" s="2">
         <v>0</v>
@@ -1145,7 +1145,7 @@
         <v>4.03</v>
       </c>
       <c r="F24" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G24" s="2">
         <v>0</v>
@@ -1174,7 +1174,7 @@
         <v>4.0599999999999996</v>
       </c>
       <c r="F25" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G25" s="2">
         <v>0</v>
@@ -1203,7 +1203,7 @@
         <v>4</v>
       </c>
       <c r="F26" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G26" s="2">
         <v>0</v>
@@ -1232,7 +1232,7 @@
         <v>4.0599999999999996</v>
       </c>
       <c r="F27" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G27" s="2">
         <v>0</v>
@@ -1261,7 +1261,7 @@
         <v>0</v>
       </c>
       <c r="F28" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G28" s="2">
         <v>246.30539999999999</v>
@@ -1290,7 +1290,7 @@
         <v>8</v>
       </c>
       <c r="F29" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G29" s="2">
         <v>0</v>
@@ -1319,7 +1319,7 @@
         <v>0</v>
       </c>
       <c r="F30" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G30" s="2">
         <v>250</v>
@@ -1348,7 +1348,7 @@
         <v>4</v>
       </c>
       <c r="F31" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G31" s="2">
         <v>0</v>
@@ -1377,7 +1377,7 @@
         <v>4.01</v>
       </c>
       <c r="F32" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G32" s="2">
         <v>0</v>
@@ -1406,7 +1406,7 @@
         <v>4.0199999999999996</v>
       </c>
       <c r="F33" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G33" s="2">
         <v>0</v>
@@ -1435,7 +1435,7 @@
         <v>4.03</v>
       </c>
       <c r="F34" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G34" s="2">
         <v>0</v>
@@ -1464,7 +1464,7 @@
         <v>4.0599999999999996</v>
       </c>
       <c r="F35" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G35" s="2">
         <v>0</v>
@@ -1493,7 +1493,7 @@
         <v>4</v>
       </c>
       <c r="F36" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G36" s="2">
         <v>0</v>
@@ -1522,7 +1522,7 @@
         <v>4.0599999999999996</v>
       </c>
       <c r="F37" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G37" s="2">
         <v>0</v>
@@ -1551,7 +1551,7 @@
         <v>8</v>
       </c>
       <c r="F38" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G38" s="2">
         <v>0</v>
@@ -1580,7 +1580,7 @@
         <v>2</v>
       </c>
       <c r="F39" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G39" s="2">
         <v>0</v>
@@ -1609,7 +1609,7 @@
         <v>3</v>
       </c>
       <c r="F40" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G40" s="2">
         <v>0</v>
@@ -1638,7 +1638,7 @@
         <v>4</v>
       </c>
       <c r="F41" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G41" s="2">
         <v>0</v>
@@ -1667,7 +1667,7 @@
         <v>5</v>
       </c>
       <c r="F42" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G42" s="2">
         <v>0</v>
@@ -1696,7 +1696,7 @@
         <v>6</v>
       </c>
       <c r="F43" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G43" s="2">
         <v>0</v>
@@ -1725,7 +1725,7 @@
         <v>7</v>
       </c>
       <c r="F44" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G44" s="2">
         <v>0</v>
@@ -1754,7 +1754,7 @@
         <v>8</v>
       </c>
       <c r="F45" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G45" s="2">
         <v>0</v>
@@ -1783,7 +1783,7 @@
         <v>2</v>
       </c>
       <c r="F46" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G46" s="2">
         <v>0</v>
@@ -1812,7 +1812,7 @@
         <v>3</v>
       </c>
       <c r="F47" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G47" s="2">
         <v>0</v>
@@ -1841,7 +1841,7 @@
         <v>4</v>
       </c>
       <c r="F48" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G48" s="2">
         <v>0</v>
@@ -1870,7 +1870,7 @@
         <v>5</v>
       </c>
       <c r="F49" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G49" s="2">
         <v>0</v>
@@ -1899,7 +1899,7 @@
         <v>6</v>
       </c>
       <c r="F50" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G50" s="2">
         <v>0</v>
@@ -1928,7 +1928,7 @@
         <v>7</v>
       </c>
       <c r="F51" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G51" s="2">
         <v>0</v>
@@ -1957,7 +1957,7 @@
         <v>8</v>
       </c>
       <c r="F52" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G52" s="2">
         <v>0</v>

</xml_diff>

<commit_message>
update 20220708 18:44 by xhx
</commit_message>
<xml_diff>
--- a/rules/rules.xlsx
+++ b/rules/rules.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20338"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7905835-6979-43B8-A38A-6A776940A44B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{610EF8A4-68FC-45E4-96B4-F146CAE6D70C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -446,7 +446,7 @@
   <dimension ref="A1:I52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -507,7 +507,7 @@
         <v>4.0599999999999996</v>
       </c>
       <c r="F2" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G2" s="2">
         <v>0</v>
@@ -536,7 +536,7 @@
         <v>8.1199999999999992</v>
       </c>
       <c r="F3" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G3" s="2">
         <v>0</v>
@@ -565,7 +565,7 @@
         <v>16.239999999999998</v>
       </c>
       <c r="F4" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G4" s="2">
         <v>0</v>
@@ -594,7 +594,7 @@
         <v>32.479999999999997</v>
       </c>
       <c r="F5" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G5" s="2">
         <v>0</v>
@@ -826,7 +826,7 @@
         <v>4</v>
       </c>
       <c r="F13" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G13" s="2">
         <v>0</v>
@@ -855,7 +855,7 @@
         <v>4.01</v>
       </c>
       <c r="F14" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G14" s="2">
         <v>0</v>
@@ -884,7 +884,7 @@
         <v>4.0199999999999996</v>
       </c>
       <c r="F15" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G15" s="2">
         <v>0</v>
@@ -913,7 +913,7 @@
         <v>4.03</v>
       </c>
       <c r="F16" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G16" s="2">
         <v>0</v>
@@ -942,7 +942,7 @@
         <v>4.0599999999999996</v>
       </c>
       <c r="F17" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G17" s="2">
         <v>0</v>
@@ -1029,7 +1029,7 @@
         <v>0</v>
       </c>
       <c r="F20" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G20" s="2">
         <v>246.30539999999999</v>
@@ -1058,7 +1058,7 @@
         <v>4</v>
       </c>
       <c r="F21" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G21" s="2">
         <v>0</v>
@@ -1087,7 +1087,7 @@
         <v>4.01</v>
       </c>
       <c r="F22" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G22" s="2">
         <v>0</v>
@@ -1116,7 +1116,7 @@
         <v>4.0199999999999996</v>
       </c>
       <c r="F23" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G23" s="2">
         <v>0</v>
@@ -1145,7 +1145,7 @@
         <v>4.03</v>
       </c>
       <c r="F24" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G24" s="2">
         <v>0</v>
@@ -1174,7 +1174,7 @@
         <v>4.0599999999999996</v>
       </c>
       <c r="F25" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G25" s="2">
         <v>0</v>
@@ -1261,7 +1261,7 @@
         <v>0</v>
       </c>
       <c r="F28" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G28" s="2">
         <v>246.30539999999999</v>
@@ -1319,7 +1319,7 @@
         <v>0</v>
       </c>
       <c r="F30" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G30" s="2">
         <v>250</v>
@@ -1348,7 +1348,7 @@
         <v>4</v>
       </c>
       <c r="F31" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G31" s="2">
         <v>0</v>
@@ -1377,7 +1377,7 @@
         <v>4.01</v>
       </c>
       <c r="F32" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G32" s="2">
         <v>0</v>
@@ -1406,7 +1406,7 @@
         <v>4.0199999999999996</v>
       </c>
       <c r="F33" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G33" s="2">
         <v>0</v>
@@ -1435,7 +1435,7 @@
         <v>4.03</v>
       </c>
       <c r="F34" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G34" s="2">
         <v>0</v>
@@ -1464,7 +1464,7 @@
         <v>4.0599999999999996</v>
       </c>
       <c r="F35" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G35" s="2">
         <v>0</v>
@@ -1580,7 +1580,7 @@
         <v>2</v>
       </c>
       <c r="F39" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G39" s="2">
         <v>0</v>
@@ -1609,7 +1609,7 @@
         <v>3</v>
       </c>
       <c r="F40" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G40" s="2">
         <v>0</v>
@@ -1638,7 +1638,7 @@
         <v>4</v>
       </c>
       <c r="F41" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G41" s="2">
         <v>0</v>
@@ -1667,7 +1667,7 @@
         <v>5</v>
       </c>
       <c r="F42" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G42" s="2">
         <v>0</v>
@@ -1696,7 +1696,7 @@
         <v>6</v>
       </c>
       <c r="F43" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G43" s="2">
         <v>0</v>
@@ -1725,7 +1725,7 @@
         <v>7</v>
       </c>
       <c r="F44" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G44" s="2">
         <v>0</v>
@@ -1754,7 +1754,7 @@
         <v>8</v>
       </c>
       <c r="F45" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G45" s="2">
         <v>0</v>

</xml_diff>

<commit_message>
update 20230419 by xhx
</commit_message>
<xml_diff>
--- a/rules/rules.xlsx
+++ b/rules/rules.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20338"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2681442B-3842-4C3A-B684-45DE2E97EE9F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7826FC96-6E6A-4540-92FB-81025A67E002}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="22">
   <si>
     <t>ICI</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -99,6 +99,10 @@
   </si>
   <si>
     <t>variance</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ISI</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -439,10 +443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H52"/>
+  <dimension ref="A1:I52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -456,7 +460,7 @@
     <col min="10" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -481,8 +485,11 @@
       <c r="H1" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -507,8 +514,11 @@
       <c r="H2" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -533,8 +543,11 @@
       <c r="H3" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -559,8 +572,11 @@
       <c r="H4" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -585,8 +601,11 @@
       <c r="H5" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -611,8 +630,11 @@
       <c r="H6" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -637,8 +659,11 @@
       <c r="H7" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -663,8 +688,11 @@
       <c r="H8" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
@@ -689,8 +717,11 @@
       <c r="H9" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
@@ -715,8 +746,11 @@
       <c r="H10" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -741,8 +775,11 @@
       <c r="H11" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
@@ -767,8 +804,11 @@
       <c r="H12" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
@@ -793,8 +833,11 @@
       <c r="H13" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I13" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
@@ -819,8 +862,11 @@
       <c r="H14" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I14" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>8</v>
       </c>
@@ -845,8 +891,11 @@
       <c r="H15" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I15" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>8</v>
       </c>
@@ -871,8 +920,11 @@
       <c r="H16" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I16" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>8</v>
       </c>
@@ -897,8 +949,11 @@
       <c r="H17" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I17" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>8</v>
       </c>
@@ -923,8 +978,11 @@
       <c r="H18" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I18" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>8</v>
       </c>
@@ -949,8 +1007,11 @@
       <c r="H19" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I19" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>8</v>
       </c>
@@ -975,8 +1036,11 @@
       <c r="H20" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I20" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>14</v>
       </c>
@@ -1001,8 +1065,11 @@
       <c r="H21" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I21" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>14</v>
       </c>
@@ -1027,8 +1094,11 @@
       <c r="H22" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I22" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>13</v>
       </c>
@@ -1053,8 +1123,11 @@
       <c r="H23" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I23" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>13</v>
       </c>
@@ -1079,8 +1152,11 @@
       <c r="H24" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I24" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>13</v>
       </c>
@@ -1105,8 +1181,11 @@
       <c r="H25" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I25" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>13</v>
       </c>
@@ -1131,8 +1210,11 @@
       <c r="H26" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I26" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>13</v>
       </c>
@@ -1157,8 +1239,11 @@
       <c r="H27" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I27" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>13</v>
       </c>
@@ -1183,8 +1268,11 @@
       <c r="H28" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I28" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>13</v>
       </c>
@@ -1209,8 +1297,11 @@
       <c r="H29" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I29" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>13</v>
       </c>
@@ -1235,8 +1326,11 @@
       <c r="H30" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I30" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>17</v>
       </c>
@@ -1261,8 +1355,11 @@
       <c r="H31" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I31" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>17</v>
       </c>
@@ -1287,8 +1384,11 @@
       <c r="H32" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I32" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>16</v>
       </c>
@@ -1313,8 +1413,11 @@
       <c r="H33" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I33" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>16</v>
       </c>
@@ -1339,8 +1442,11 @@
       <c r="H34" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I34" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>16</v>
       </c>
@@ -1365,8 +1471,11 @@
       <c r="H35" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I35" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>16</v>
       </c>
@@ -1391,8 +1500,11 @@
       <c r="H36" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I36" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>16</v>
       </c>
@@ -1417,8 +1529,11 @@
       <c r="H37" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I37" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>16</v>
       </c>
@@ -1443,8 +1558,11 @@
       <c r="H38" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I38" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>18</v>
       </c>
@@ -1469,8 +1587,11 @@
       <c r="H39" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I39" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>18</v>
       </c>
@@ -1495,8 +1616,11 @@
       <c r="H40" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I40" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>18</v>
       </c>
@@ -1521,8 +1645,11 @@
       <c r="H41" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I41" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>18</v>
       </c>
@@ -1547,8 +1674,11 @@
       <c r="H42" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I42" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>18</v>
       </c>
@@ -1573,8 +1703,11 @@
       <c r="H43" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I43" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>18</v>
       </c>
@@ -1599,8 +1732,11 @@
       <c r="H44" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I44" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>18</v>
       </c>
@@ -1625,8 +1761,11 @@
       <c r="H45" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I45" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>18</v>
       </c>
@@ -1651,8 +1790,11 @@
       <c r="H46" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I46" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>18</v>
       </c>
@@ -1677,8 +1819,11 @@
       <c r="H47" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I47" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>18</v>
       </c>
@@ -1703,8 +1848,11 @@
       <c r="H48" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I48" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>18</v>
       </c>
@@ -1729,8 +1877,11 @@
       <c r="H49" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I49" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>18</v>
       </c>
@@ -1755,8 +1906,11 @@
       <c r="H50" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I50" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>18</v>
       </c>
@@ -1781,8 +1935,11 @@
       <c r="H51" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I51" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>18</v>
       </c>
@@ -1806,6 +1963,9 @@
       </c>
       <c r="H52" s="2" t="b">
         <v>0</v>
+      </c>
+      <c r="I52" s="2">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>